<commit_message>
just for recording: refactor for use php-typescript-kotlin shared definition sheets.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13D23E6-8429-6747-AB7D-4C776EC6A6FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D89E9F-DB13-B843-A90A-EF61F20CF3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,6 @@
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="accessScope">config!$B$4:$B$6</definedName>
     <definedName name="accessScope2">config!$B$4:$B$5</definedName>
@@ -44,12 +41,14 @@
     <definedName name="必須" localSheetId="1">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -194,10 +193,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>PhpSample</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>dateField1</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -294,6 +289,10 @@
   </si>
   <si>
     <t>○</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>PhpSample</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -829,12 +828,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -864,6 +857,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -949,21 +948,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="valueObject"/>
-      <sheetName val="config"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1294,7 +1278,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1340,7 +1324,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
@@ -1383,12 +1367,12 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:9" s="35" customFormat="1">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44" t="s">
         <v>47</v>
-      </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46" t="s">
-        <v>48</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -1396,12 +1380,12 @@
       <c r="G10"/>
     </row>
     <row r="11" spans="1:9" s="35" customFormat="1">
-      <c r="A11" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46" t="s">
+      <c r="A11" s="42" t="s">
         <v>48</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44" t="s">
+        <v>47</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -1467,33 +1451,33 @@
       <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="42"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
       <c r="G18" s="18"/>
       <c r="H18" s="31"/>
       <c r="I18" s="15"/>
@@ -1509,7 +1493,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>19</v>
@@ -1589,10 +1573,10 @@
         <v>23</v>
       </c>
       <c r="D23" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>43</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
@@ -1703,14 +1687,14 @@
         <v>11</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -1723,10 +1707,10 @@
         <v>12</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -1808,78 +1792,78 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="49" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="49" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="49" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="256" width="8.83203125" style="49" customWidth="1"/>
-    <col min="257" max="16384" width="10.83203125" style="49"/>
+    <col min="1" max="3" width="8.83203125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="256" width="8.83203125" style="47" customWidth="1"/>
+    <col min="257" max="16384" width="10.83203125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="48" t="s">
+      <c r="M1" s="46"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="48"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="B3" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="50" t="s">
+      <c r="H3" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="J3" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="50" t="s">
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="J4" s="50"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="51" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="B4" s="51"/>
-      <c r="D4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="J4" s="52"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="B5" s="53" t="s">
+      <c r="D5" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="54" t="s">
-        <v>56</v>
+      <c r="F5" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="55"/>
+      <c r="B6" s="53"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
2.1.3: SimpleName ArrayList, List, HashMap, Map types are converted into CanonicalName to import java.uti package.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D89E9F-DB13-B843-A90A-EF61F20CF3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A39FF1-E3B8-1E46-9951-4F7152F81188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>クラス名</t>
   </si>
@@ -293,6 +293,72 @@
   </si>
   <si>
     <t>PhpSample</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>arrayList</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ArrayList</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>CanonicalNameに置き換えられて、import文が自動生成されることを確認する</t>
+    <rPh sb="14" eb="15">
+      <t xml:space="preserve">オキカエラレテ </t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t xml:space="preserve">ジドウ </t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t xml:space="preserve">カクニンスル </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>list</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>List</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>hashMap</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>HashMap</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>総称型</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ソウショウガタ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Long, String</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -763,7 +829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -862,6 +928,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1275,50 +1345,51 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="23.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28" style="1" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="2" max="5" width="23.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28" style="1" customWidth="1"/>
+    <col min="9" max="9" width="33.33203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19">
+    <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1326,10 +1397,11 @@
       <c r="C6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="D6" s="12"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1337,10 +1409,11 @@
       <c r="C7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="D7" s="56"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1351,9 +1424,10 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="G8" s="12"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1364,9 +1438,10 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" s="35" customFormat="1">
+      <c r="G9" s="12"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" s="35" customFormat="1">
       <c r="A10" s="42" t="s">
         <v>46</v>
       </c>
@@ -1374,12 +1449,13 @@
       <c r="C10" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D10"/>
+      <c r="D10" s="57"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-    </row>
-    <row r="11" spans="1:9" s="35" customFormat="1">
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:10" s="35" customFormat="1">
       <c r="A11" s="42" t="s">
         <v>48</v>
       </c>
@@ -1387,57 +1463,62 @@
       <c r="C11" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D11"/>
+      <c r="D11" s="57"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="35"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="35"/>
       <c r="H13" s="35"/>
       <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="35"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="37" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="35"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="35"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15" s="35"/>
+      <c r="G15"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="35"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1447,10 +1528,11 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" ht="13.5" customHeight="1">
+      <c r="H16" s="14"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" ht="13.5" customHeight="1">
       <c r="A17" s="55" t="s">
         <v>4</v>
       </c>
@@ -1461,28 +1543,32 @@
         <v>6</v>
       </c>
       <c r="D17" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="F17" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="G17" s="54"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="55"/>
       <c r="B18" s="55"/>
       <c r="C18" s="54"/>
       <c r="D18" s="54"/>
       <c r="E18" s="54"/>
       <c r="F18" s="54"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="G18" s="54"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="19">
         <v>1</v>
       </c>
@@ -1492,20 +1578,21 @@
       <c r="C19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="F19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="H19" s="22"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="19">
-        <f t="shared" ref="A20:A30" si="0">A19+1</f>
+        <f t="shared" ref="A20:A34" si="0">A19+1</f>
         <v>2</v>
       </c>
       <c r="B20" s="20" t="s">
@@ -1515,13 +1602,14 @@
         <v>25</v>
       </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="22"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="19">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1532,18 +1620,19 @@
       <c r="C21" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="21"/>
+      <c r="E21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="F21" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1555,13 +1644,14 @@
         <v>17</v>
       </c>
       <c r="D22" s="21"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="22"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1572,18 +1662,19 @@
       <c r="C23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="21"/>
+      <c r="E23" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="F23" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="15"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1596,12 +1687,13 @@
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
+      <c r="F24" s="21"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="15"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="19">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1612,18 +1704,19 @@
       <c r="C25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="21"/>
+      <c r="E25" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="F25" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="15"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="19">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1636,12 +1729,13 @@
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
-      <c r="F26" s="22"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="15"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1652,18 +1746,19 @@
       <c r="C27" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="F27" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="15"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1676,12 +1771,13 @@
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="15"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="H28" s="22"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="19">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1692,16 +1788,17 @@
       <c r="C29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="21" t="s">
+      <c r="D29" s="21"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="15"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="19">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1714,62 +1811,147 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
+      <c r="F30" s="21"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="15"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="E31" s="21"/>
-      <c r="F31" s="22"/>
+      <c r="F31" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G31" s="22"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="15"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="19">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="E32" s="21"/>
-      <c r="F32" s="22"/>
+      <c r="F32" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G32" s="22"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="25"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="15"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E17:F18"/>
+  <mergeCells count="6">
+    <mergeCell ref="F17:G18"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="D17:D18"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D49" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E52" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{5C3FAC47-29F4-8A43-89F5-93527DDFC948}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:D10" xr:uid="{5C3FAC47-29F4-8A43-89F5-93527DDFC948}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{EC2D82BC-D8A5-C34C-B774-4F979A3C0491}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:D11" xr:uid="{EC2D82BC-D8A5-C34C-B774-4F979A3C0491}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>